<commit_message>
a few corrections to the transit boardings files for the correct ids
it's still not completely fixed!
</commit_message>
<xml_diff>
--- a/inputs/ObservedBoardings.xlsx
+++ b/inputs/ObservedBoardings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11310"/>
+    <workbookView xWindow="5655" yWindow="945" windowWidth="18195" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="AM" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="443">
   <si>
     <t>Route</t>
   </si>
@@ -1208,12 +1208,6 @@
     <t>ET702</t>
   </si>
   <si>
-    <t>ST001</t>
-  </si>
-  <si>
-    <t>ST003</t>
-  </si>
-  <si>
     <t>ST011</t>
   </si>
   <si>
@@ -1341,6 +1335,15 @@
   </si>
   <si>
     <t>WFVSW</t>
+  </si>
+  <si>
+    <t>RLCRL</t>
+  </si>
+  <si>
+    <t>RLLRL</t>
+  </si>
+  <si>
+    <t>RLMNR</t>
   </si>
 </sst>
 </file>
@@ -1705,7 +1708,7 @@
   <dimension ref="A1:C493"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
-      <selection activeCell="E428" sqref="E428"/>
+      <selection activeCell="A419" sqref="A419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -5010,7 +5013,7 @@
     </row>
     <row r="374" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B374" s="3">
         <v>770.46738732584618</v>
@@ -5018,7 +5021,7 @@
     </row>
     <row r="375" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B375" s="3">
         <v>825.79951282012041</v>
@@ -5026,7 +5029,7 @@
     </row>
     <row r="376" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B376" s="3">
         <v>811.5</v>
@@ -5034,7 +5037,7 @@
     </row>
     <row r="377" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B377" s="3">
         <v>356.58758311540225</v>
@@ -5043,7 +5046,7 @@
     </row>
     <row r="378" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B378" s="3">
         <v>419.78506038345648</v>
@@ -5051,7 +5054,7 @@
     </row>
     <row r="379" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B379" s="3">
         <v>334.8</v>
@@ -5059,7 +5062,7 @@
     </row>
     <row r="380" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B380" s="3">
         <v>1801.2</v>
@@ -5067,7 +5070,7 @@
     </row>
     <row r="381" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B381" s="3">
         <v>1999.2</v>
@@ -5075,7 +5078,7 @@
     </row>
     <row r="382" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B382" s="3">
         <v>388.2</v>
@@ -5083,7 +5086,7 @@
     </row>
     <row r="383" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B383" s="3">
         <v>205.4</v>
@@ -5091,7 +5094,7 @@
     </row>
     <row r="384" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B384" s="3">
         <v>260.3</v>
@@ -5099,7 +5102,7 @@
     </row>
     <row r="385" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B385" s="3">
         <v>375.2</v>
@@ -5107,7 +5110,7 @@
     </row>
     <row r="386" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B386" s="3">
         <v>666.2</v>
@@ -5115,7 +5118,7 @@
     </row>
     <row r="387" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B387" s="3">
         <v>667.9431511888921</v>
@@ -5123,7 +5126,7 @@
     </row>
     <row r="388" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B388" s="3">
         <v>505.1</v>
@@ -5131,7 +5134,7 @@
     </row>
     <row r="389" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B389" s="3">
         <v>250.82981347144971</v>
@@ -5331,7 +5334,7 @@
     </row>
     <row r="414" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>397</v>
+        <v>440</v>
       </c>
       <c r="B414" s="3">
         <v>4127.568181818182</v>
@@ -5339,7 +5342,7 @@
     </row>
     <row r="415" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>398</v>
+        <v>440</v>
       </c>
       <c r="B415" s="3">
         <v>548.72727272727275</v>
@@ -5347,7 +5350,7 @@
     </row>
     <row r="416" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>399</v>
+        <v>441</v>
       </c>
       <c r="B416" s="3">
         <v>2840</v>
@@ -5355,7 +5358,7 @@
     </row>
     <row r="417" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
-        <v>400</v>
+        <v>441</v>
       </c>
       <c r="B417" s="3">
         <v>552.41</v>
@@ -5363,7 +5366,7 @@
     </row>
     <row r="418" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>401</v>
+        <v>442</v>
       </c>
       <c r="B418" s="3">
         <v>1596</v>
@@ -5371,7 +5374,7 @@
     </row>
     <row r="419" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B419" s="3">
         <v>260</v>
@@ -5379,7 +5382,7 @@
     </row>
     <row r="420" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B420" s="3">
         <v>393.99</v>
@@ -5387,7 +5390,7 @@
     </row>
     <row r="421" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B421" s="3">
         <v>164.91</v>
@@ -5395,7 +5398,7 @@
     </row>
     <row r="422" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B422" s="3">
         <v>43</v>
@@ -5403,7 +5406,7 @@
     </row>
     <row r="423" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B423" s="3">
         <v>16</v>
@@ -5411,7 +5414,7 @@
     </row>
     <row r="424" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B424" s="3">
         <v>594</v>
@@ -5419,7 +5422,7 @@
     </row>
     <row r="425" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B425" s="3">
         <v>195</v>
@@ -5427,7 +5430,7 @@
     </row>
     <row r="426" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A426" s="7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B426" s="6">
         <f>1817926/365</f>
@@ -5436,7 +5439,7 @@
     </row>
     <row r="427" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A427" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B427" s="6">
         <f>319765/365</f>
@@ -5445,7 +5448,7 @@
     </row>
     <row r="428" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A428" s="7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B428" s="6">
         <f>25741/365</f>
@@ -5454,7 +5457,7 @@
     </row>
     <row r="429" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A429" s="7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B429" s="6">
         <f>4304850/365</f>
@@ -5463,7 +5466,7 @@
     </row>
     <row r="430" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A430" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B430" s="6">
         <f>1665013/365</f>
@@ -5472,7 +5475,7 @@
     </row>
     <row r="431" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A431" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B431" s="6">
         <v>0</v>
@@ -5480,7 +5483,7 @@
     </row>
     <row r="432" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A432" s="7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B432" s="6">
         <f>824982/365</f>
@@ -5489,7 +5492,7 @@
     </row>
     <row r="433" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A433" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B433" s="6">
         <f>319765/365</f>
@@ -5523,7 +5526,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6368,7 +6371,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B107" s="3">
         <v>11.7</v>
@@ -6728,7 +6731,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B152" s="3">
         <v>260</v>
@@ -7248,7 +7251,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B217" s="3">
         <v>16.070649673905116</v>
@@ -7272,7 +7275,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B220" s="3">
         <v>20.157888901054879</v>
@@ -7288,7 +7291,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B222" s="3">
         <v>62.064490330085789</v>
@@ -7312,7 +7315,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B225" s="3">
         <v>37.159761912095682</v>
@@ -7336,7 +7339,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B228" s="3">
         <v>154.53025193140991</v>
@@ -7560,7 +7563,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B256" s="3">
         <v>44</v>
@@ -7600,7 +7603,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B261" s="3">
         <v>462.51000000000005</v>
@@ -7608,7 +7611,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B262" s="3">
         <v>193.59</v>
@@ -7616,7 +7619,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B263" s="3">
         <v>238</v>
@@ -7624,7 +7627,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B264" s="3">
         <v>30</v>
@@ -7632,7 +7635,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B265" s="3">
         <v>1869</v>
@@ -7640,7 +7643,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B266" s="3">
         <v>1235</v>
@@ -7648,7 +7651,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B267" s="3">
         <v>1212.316</v>
@@ -7656,7 +7659,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B268" s="3">
         <v>7079</v>
@@ -7664,7 +7667,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B269" s="3">
         <v>754.62200313004985</v>
@@ -7672,7 +7675,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B270" s="3">
         <v>808.81617158519509</v>
@@ -7680,7 +7683,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B271" s="3">
         <v>1027.8</v>
@@ -7688,7 +7691,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B272" s="3">
         <v>349.2540251389575</v>
@@ -7696,7 +7699,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B273" s="3">
         <v>411.15178703425204</v>
@@ -7704,7 +7707,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B274" s="3">
         <v>437.7</v>
@@ -7712,7 +7715,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B275" s="3">
         <v>1703.9</v>
@@ -7720,7 +7723,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="7" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B276" s="3">
         <v>1863.5</v>
@@ -7728,7 +7731,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B277" s="3">
         <v>1095.5999999999999</v>
@@ -7736,7 +7739,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="7" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B278" s="3">
         <v>3.2</v>
@@ -7744,7 +7747,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B279" s="3">
         <v>58.7</v>
@@ -7752,7 +7755,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B280" s="3">
         <v>571.1</v>
@@ -7760,7 +7763,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B281" s="3">
         <v>431.6</v>
@@ -7768,7 +7771,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B282" s="3">
         <v>654.20627403400908</v>
@@ -7776,7 +7779,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B283" s="3">
         <v>2.9</v>
@@ -7784,7 +7787,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B284" s="3">
         <v>245.67126318418863</v>
@@ -7984,7 +7987,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B309" s="3">
         <v>2310</v>
@@ -7992,7 +7995,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B310" s="6">
         <f>1817926/365</f>
@@ -8001,7 +8004,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B311" s="6">
         <f>319765/365</f>
@@ -8010,7 +8013,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B312" s="6">
         <f>25741/365</f>
@@ -8019,7 +8022,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B313" s="6">
         <f>4304850/365</f>
@@ -8028,7 +8031,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B314" s="6">
         <f>1665013/365</f>
@@ -8037,7 +8040,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B315" s="6">
         <v>0</v>
@@ -8045,7 +8048,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B316" s="6">
         <f>824982/365</f>
@@ -8054,7 +8057,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B317" s="6">
         <f>319765/365</f>

</xml_diff>

<commit_message>
Filling a few missing numbers on the observed boardings spreadsheet
</commit_message>
<xml_diff>
--- a/inputs/ObservedBoardings.xlsx
+++ b/inputs/ObservedBoardings.xlsx
@@ -3034,7 +3034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D443"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A414" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -9221,8 +9221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D443"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="D351" sqref="D351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14798,8 +14798,7 @@
         <v>772</v>
       </c>
       <c r="D401">
-        <f>D$513*AM!$R386</f>
-        <v>0</v>
+        <v>770</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -14813,8 +14812,7 @@
         <v>774</v>
       </c>
       <c r="D402">
-        <f>D$513*AM!$R387</f>
-        <v>0</v>
+        <v>809</v>
       </c>
     </row>
     <row r="403" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -14856,8 +14854,7 @@
         <v>780</v>
       </c>
       <c r="D405">
-        <f>D$513*AM!$R390</f>
-        <v>0</v>
+        <v>349</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
@@ -14871,8 +14868,7 @@
         <v>782</v>
       </c>
       <c r="D406">
-        <f>D$513*AM!$R391</f>
-        <v>0</v>
+        <v>420</v>
       </c>
     </row>
     <row r="407" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -14998,8 +14994,7 @@
         <v>800</v>
       </c>
       <c r="D415">
-        <f>D$513*AM!$R400</f>
-        <v>0</v>
+        <v>654</v>
       </c>
     </row>
     <row r="416" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -15027,8 +15022,7 @@
         <v>804</v>
       </c>
       <c r="D417">
-        <f>D$513*AM!$R402</f>
-        <v>0</v>
+        <v>245</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
@@ -15042,8 +15036,7 @@
         <v>806</v>
       </c>
       <c r="D418">
-        <f>D$513*AM!$R403</f>
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
@@ -15057,8 +15050,7 @@
         <v>808</v>
       </c>
       <c r="D419">
-        <f>D$513*AM!$R404</f>
-        <v>0</v>
+        <v>467</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
@@ -15072,8 +15064,7 @@
         <v>810</v>
       </c>
       <c r="D420">
-        <f>D$513*AM!$R405</f>
-        <v>0</v>
+        <v>224</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
@@ -15101,8 +15092,7 @@
         <v>814</v>
       </c>
       <c r="D422">
-        <f>D$513*AM!$R407</f>
-        <v>0</v>
+        <v>473</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
@@ -15130,8 +15120,7 @@
         <v>818</v>
       </c>
       <c r="D424">
-        <f>D$513*AM!$R409</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="425" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -15397,8 +15386,7 @@
         <v>864</v>
       </c>
       <c r="D443" s="3">
-        <f>0.33*AM!K432</f>
-        <v>0</v>
+        <v>2310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>